<commit_message>
Add some instruction into VM and initial the interrupt functionality. Besides, I fix some problem in makefile, which is the .cpp file hadn't been added into dependencies.
</commit_message>
<xml_diff>
--- a/ZPC-ISA.xlsx
+++ b/ZPC-ISA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sea\Documents\Tencent Files\597651954\FileRecv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education\My Resource\AaI\SerenityTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="286">
   <si>
     <t xml:space="preserve">格式 </t>
   </si>
@@ -1924,11 +1924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80:N115"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2400,7 +2399,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="10" spans="1:16" ht="16.2" thickBot="1">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -2446,7 +2445,7 @@
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="11" spans="1:16" ht="16.2" thickBot="1">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -2492,7 +2491,7 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="12" spans="1:16" ht="16.2" thickBot="1">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -2538,7 +2537,7 @@
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="13" spans="1:16" ht="16.2" thickBot="1">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -2584,7 +2583,7 @@
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
     </row>
-    <row r="14" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="14" spans="1:16" ht="16.2" thickBot="1">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -2630,7 +2629,7 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="15" spans="1:16" ht="16.2" thickBot="1">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -2676,7 +2675,7 @@
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="16" spans="1:16" ht="16.2" thickBot="1">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -2722,7 +2721,7 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="17" spans="1:16" ht="16.2" thickBot="1">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -2768,7 +2767,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="18" spans="1:16" ht="16.2" thickBot="1">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -3314,7 +3313,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="29" spans="1:16" ht="16.2" thickBot="1">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -3360,7 +3359,7 @@
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
     </row>
-    <row r="30" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="30" spans="1:16" ht="16.2" thickBot="1">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -3406,7 +3405,7 @@
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
     </row>
-    <row r="31" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="31" spans="1:16" ht="16.2" thickBot="1">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -3452,7 +3451,7 @@
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="32" spans="1:16" ht="16.2" thickBot="1">
       <c r="A32" s="10">
         <v>30</v>
       </c>
@@ -3498,7 +3497,7 @@
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="33" spans="1:16" ht="16.2" thickBot="1">
       <c r="A33" s="10">
         <v>31</v>
       </c>
@@ -3694,7 +3693,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="37" spans="1:16" ht="16.2" thickBot="1">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -3740,7 +3739,7 @@
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
-    <row r="38" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="38" spans="1:16" ht="16.2" thickBot="1">
       <c r="A38" s="10">
         <v>36</v>
       </c>
@@ -3786,7 +3785,7 @@
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
     </row>
-    <row r="39" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="39" spans="1:16" ht="16.2" thickBot="1">
       <c r="A39" s="10">
         <v>37</v>
       </c>
@@ -4332,7 +4331,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="50" spans="1:16" ht="16.2" thickBot="1">
       <c r="A50" s="10">
         <v>48</v>
       </c>
@@ -4378,7 +4377,7 @@
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
     </row>
-    <row r="51" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="51" spans="1:16" ht="16.2" thickBot="1">
       <c r="A51" s="10">
         <v>49</v>
       </c>
@@ -4424,7 +4423,7 @@
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
     </row>
-    <row r="52" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="52" spans="1:16" ht="16.2" thickBot="1">
       <c r="A52" s="10">
         <v>50</v>
       </c>
@@ -4520,7 +4519,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="54" spans="1:16" ht="16.2" thickBot="1">
       <c r="A54" s="10">
         <v>52</v>
       </c>
@@ -4666,7 +4665,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="57" spans="1:16" ht="16.2" thickBot="1">
       <c r="A57" s="10">
         <v>55</v>
       </c>
@@ -4712,7 +4711,7 @@
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
     </row>
-    <row r="58" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="58" spans="1:16" ht="16.2" thickBot="1">
       <c r="A58" s="10">
         <v>56</v>
       </c>
@@ -4760,7 +4759,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="16.2" hidden="1" thickBot="1">
+    <row r="59" spans="1:16" ht="16.2" thickBot="1">
       <c r="A59" s="10">
         <v>57</v>
       </c>
@@ -4908,1489 +4907,547 @@
     </row>
     <row r="79" spans="2:14" ht="15" thickBot="1"/>
     <row r="80" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B80" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="H80" s="6">
-        <v>0</v>
-      </c>
-      <c r="I80" s="6">
-        <v>0</v>
-      </c>
-      <c r="J80" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K80" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L80" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="M80" s="6">
-        <v>0</v>
-      </c>
-      <c r="N80" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
     </row>
     <row r="81" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B81" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G81" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="H81" s="6">
-        <v>0</v>
-      </c>
-      <c r="I81" s="6">
-        <v>0</v>
-      </c>
-      <c r="J81" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K81" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L81" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="M81" s="6">
-        <v>2</v>
-      </c>
-      <c r="N81" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
     </row>
     <row r="82" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B82" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="H82" s="6">
-        <v>0</v>
-      </c>
-      <c r="I82" s="6">
-        <v>0</v>
-      </c>
-      <c r="J82" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K82" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L82" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="M82" s="6">
-        <v>3</v>
-      </c>
-      <c r="N82" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
     </row>
     <row r="83" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B83" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="H83" s="6">
-        <v>0</v>
-      </c>
-      <c r="I83" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J83" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K83" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L83" s="6">
-        <v>0</v>
-      </c>
-      <c r="M83" s="6">
-        <v>4</v>
-      </c>
-      <c r="N83" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
     </row>
     <row r="84" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B84" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="H84" s="6">
-        <v>0</v>
-      </c>
-      <c r="I84" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J84" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K84" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L84" s="6">
-        <v>0</v>
-      </c>
-      <c r="M84" s="6">
-        <v>6</v>
-      </c>
-      <c r="N84" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
     </row>
     <row r="85" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B85" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="F85" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="H85" s="6">
-        <v>0</v>
-      </c>
-      <c r="I85" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J85" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K85" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L85" s="6">
-        <v>0</v>
-      </c>
-      <c r="M85" s="6">
-        <v>7</v>
-      </c>
-      <c r="N85" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
     </row>
     <row r="86" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B86" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="F86" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G86" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H86" s="6">
-        <v>0</v>
-      </c>
-      <c r="I86" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J86" s="6">
-        <v>0</v>
-      </c>
-      <c r="K86" s="6">
-        <v>0</v>
-      </c>
-      <c r="L86" s="6">
-        <v>0</v>
-      </c>
-      <c r="M86" s="6">
-        <v>8</v>
-      </c>
-      <c r="N86" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="6"/>
+      <c r="N86" s="6"/>
     </row>
     <row r="87" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B87" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G87" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H87" s="6">
-        <v>0</v>
-      </c>
-      <c r="I87" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J87" s="6">
-        <v>0</v>
-      </c>
-      <c r="K87" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L87" s="6">
-        <v>0</v>
-      </c>
-      <c r="M87" s="6">
-        <v>9</v>
-      </c>
-      <c r="N87" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
     </row>
     <row r="88" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B88" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H88" s="6">
-        <v>0</v>
-      </c>
-      <c r="I88" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J88" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K88" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L88" s="6">
-        <v>0</v>
-      </c>
-      <c r="M88" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="N88" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="6"/>
+      <c r="M88" s="6"/>
+      <c r="N88" s="6"/>
     </row>
     <row r="89" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B89" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H89" s="6">
-        <v>0</v>
-      </c>
-      <c r="I89" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J89" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K89" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L89" s="6">
-        <v>0</v>
-      </c>
-      <c r="M89" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="N89" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="6"/>
+      <c r="M89" s="6"/>
+      <c r="N89" s="6"/>
     </row>
     <row r="90" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B90" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F90" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G90" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H90" s="6">
-        <v>0</v>
-      </c>
-      <c r="I90" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J90" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K90" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L90" s="6">
-        <v>0</v>
-      </c>
-      <c r="M90" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="N90" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="6"/>
+      <c r="M90" s="6"/>
+      <c r="N90" s="6"/>
     </row>
     <row r="91" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B91" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F91" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G91" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H91" s="6">
-        <v>0</v>
-      </c>
-      <c r="I91" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J91" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K91" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L91" s="6">
-        <v>0</v>
-      </c>
-      <c r="M91" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="N91" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="6"/>
+      <c r="N91" s="6"/>
     </row>
     <row r="92" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B92" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G92" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H92" s="6">
-        <v>0</v>
-      </c>
-      <c r="I92" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J92" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K92" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L92" s="6">
-        <v>0</v>
-      </c>
-      <c r="M92" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N92" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="6"/>
+      <c r="M92" s="6"/>
+      <c r="N92" s="6"/>
     </row>
     <row r="93" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B93" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G93" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H93" s="6">
-        <v>0</v>
-      </c>
-      <c r="I93" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J93" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K93" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L93" s="6">
-        <v>0</v>
-      </c>
-      <c r="M93" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="N93" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
     </row>
     <row r="94" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B94" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="F94" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G94" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H94" s="6">
-        <v>0</v>
-      </c>
-      <c r="I94" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J94" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K94" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L94" s="6">
-        <v>0</v>
-      </c>
-      <c r="M94" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="N94" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
     </row>
     <row r="95" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B95" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G95" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H95" s="6">
-        <v>0</v>
-      </c>
-      <c r="I95" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J95" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K95" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L95" s="6">
-        <v>0</v>
-      </c>
-      <c r="M95" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="N95" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
+      <c r="M95" s="6"/>
+      <c r="N95" s="6"/>
     </row>
     <row r="96" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B96" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="E96" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G96" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H96" s="6">
-        <v>0</v>
-      </c>
-      <c r="I96" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J96" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K96" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L96" s="6">
-        <v>0</v>
-      </c>
-      <c r="M96" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="N96" s="6" t="s">
-        <v>221</v>
-      </c>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
     </row>
     <row r="97" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B97" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="E97" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="F97" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G97" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H97" s="6">
-        <v>0</v>
-      </c>
-      <c r="I97" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J97" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K97" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L97" s="6">
-        <v>0</v>
-      </c>
-      <c r="M97" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="N97" s="6" t="s">
-        <v>224</v>
-      </c>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="6"/>
+      <c r="M97" s="6"/>
+      <c r="N97" s="6"/>
     </row>
     <row r="98" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B98" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="F98" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G98" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H98" s="6">
-        <v>2</v>
-      </c>
-      <c r="I98" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J98" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="K98" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="L98" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M98" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N98" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="6"/>
+      <c r="N98" s="6"/>
     </row>
     <row r="99" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B99" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D99" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F99" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G99" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H99" s="6">
-        <v>3</v>
-      </c>
-      <c r="I99" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J99" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="K99" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="L99" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M99" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N99" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="6"/>
+      <c r="M99" s="6"/>
+      <c r="N99" s="6"/>
     </row>
     <row r="100" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B100" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D100" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F100" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G100" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H100" s="6">
-        <v>4</v>
-      </c>
-      <c r="I100" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J100" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K100" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L100" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M100" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N100" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="6"/>
+      <c r="M100" s="6"/>
+      <c r="N100" s="6"/>
     </row>
     <row r="101" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B101" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F101" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G101" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H101" s="6">
-        <v>8</v>
-      </c>
-      <c r="I101" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J101" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K101" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L101" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M101" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N101" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="6"/>
+      <c r="M101" s="6"/>
+      <c r="N101" s="6"/>
     </row>
     <row r="102" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B102" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E102" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F102" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G102" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H102" s="6">
-        <v>9</v>
-      </c>
-      <c r="I102" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J102" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K102" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L102" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M102" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N102" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="6"/>
+      <c r="N102" s="6"/>
     </row>
     <row r="103" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B103" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F103" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G103" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H103" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="I103" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J103" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K103" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L103" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M103" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N103" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="6"/>
+      <c r="M103" s="6"/>
+      <c r="N103" s="6"/>
     </row>
     <row r="104" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B104" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E104" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G104" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H104" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="I104" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J104" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K104" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L104" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M104" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N104" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+      <c r="K104" s="6"/>
+      <c r="L104" s="6"/>
+      <c r="M104" s="6"/>
+      <c r="N104" s="6"/>
     </row>
     <row r="105" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B105" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E105" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H105" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I105" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J105" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K105" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L105" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M105" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N105" s="6" t="s">
-        <v>266</v>
-      </c>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="6"/>
+      <c r="M105" s="6"/>
+      <c r="N105" s="6"/>
     </row>
     <row r="106" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B106" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="D106" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="E106" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="F106" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G106" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H106" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="I106" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="J106" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="K106" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="L106" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M106" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N106" s="6" t="s">
-        <v>266</v>
-      </c>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="6"/>
     </row>
     <row r="107" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B107" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D107" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E107" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F107" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G107" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H107" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="I107" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J107" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K107" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L107" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M107" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N107" s="6" t="s">
-        <v>266</v>
-      </c>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="6"/>
+      <c r="M107" s="6"/>
+      <c r="N107" s="6"/>
     </row>
     <row r="108" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B108" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D108" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="F108" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G108" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H108" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I108" s="6">
-        <v>0</v>
-      </c>
-      <c r="J108" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K108" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L108" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M108" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N108" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="6"/>
+      <c r="N108" s="6"/>
     </row>
     <row r="109" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B109" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E109" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="F109" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="H109" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="I109" s="6">
-        <v>0</v>
-      </c>
-      <c r="J109" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K109" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L109" s="6">
-        <v>0</v>
-      </c>
-      <c r="M109" s="6">
-        <v>0</v>
-      </c>
-      <c r="N109" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="6"/>
+      <c r="M109" s="6"/>
+      <c r="N109" s="6"/>
     </row>
     <row r="110" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B110" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C110" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E110" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="F110" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G110" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="H110" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="I110" s="6">
-        <v>4</v>
-      </c>
-      <c r="J110" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K110" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L110" s="6">
-        <v>0</v>
-      </c>
-      <c r="M110" s="6">
-        <v>0</v>
-      </c>
-      <c r="N110" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6"/>
+      <c r="M110" s="6"/>
+      <c r="N110" s="6"/>
     </row>
     <row r="111" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B111" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="E111" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="F111" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G111" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H111" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="I111" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J111" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K111" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L111" s="6">
-        <v>0</v>
-      </c>
-      <c r="M111" s="6">
-        <v>2</v>
-      </c>
-      <c r="N111" s="6" t="s">
-        <v>281</v>
-      </c>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="6"/>
+      <c r="M111" s="6"/>
+      <c r="N111" s="6"/>
     </row>
     <row r="112" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B112" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E112" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F112" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G112" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H112" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I112" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J112" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K112" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L112" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M112" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N112" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B112" s="6"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+      <c r="J112" s="6"/>
+      <c r="K112" s="6"/>
+      <c r="L112" s="6"/>
+      <c r="M112" s="6"/>
+      <c r="N112" s="6"/>
     </row>
     <row r="113" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B113" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E113" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F113" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G113" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H113" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I113" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J113" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K113" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L113" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M113" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N113" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+      <c r="K113" s="6"/>
+      <c r="L113" s="6"/>
+      <c r="M113" s="6"/>
+      <c r="N113" s="6"/>
     </row>
     <row r="114" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B114" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E114" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F114" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H114" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I114" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J114" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K114" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L114" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M114" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N114" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="6"/>
+      <c r="K114" s="6"/>
+      <c r="L114" s="6"/>
+      <c r="M114" s="6"/>
+      <c r="N114" s="6"/>
     </row>
     <row r="115" spans="2:14" ht="16.2" thickBot="1">
-      <c r="B115" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E115" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F115" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H115" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="I115" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J115" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K115" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L115" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M115" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N115" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="6"/>
+      <c r="M115" s="6"/>
+      <c r="N115" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="O1:O61">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="O1:O61"/>
   <sortState ref="A2:P61">
     <sortCondition ref="H2:H61"/>
     <sortCondition ref="M2:M61"/>

</xml_diff>